<commit_message>
Added form duration automation
</commit_message>
<xml_diff>
--- a/Modelling Assumptions.xlsx
+++ b/Modelling Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0303D1-FE94-4663-BE05-BCD372077C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89396FEB-36E9-4343-AD88-5D44F7126F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{E25DF9D1-20AB-4A51-A180-B8B0280A2DA6}"/>
+    <workbookView xWindow="11168" yWindow="0" windowWidth="11415" windowHeight="14362" xr2:uid="{E25DF9D1-20AB-4A51-A180-B8B0280A2DA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,6 +241,9 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="NoOrbChaning"/>
       <sheetName val="RainbowOrbChanging"/>
@@ -574,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D2794A-FB54-4470-B8D2-C9DC8DCEEBF3}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>